<commit_message>
Bug fix & New features: Bug fixes that allow adding a bird to not existing cage Bug fixed that after showing the error of the same bird's serial number, files didn't close Added "Add new cage" option
</commit_message>
<xml_diff>
--- a/FinalQA Project/Birds habitat.xlsx
+++ b/FinalQA Project/Birds habitat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\source\repos\FinalQA Project\FinalQA Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\Source\Repos\FinalQA Project\FinalQA Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A4F8EE-CB7A-47D1-A689-A7F9D7259547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4829A49-1B99-46D0-AF2D-89DA8246846C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3636" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birds" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Length</t>
   </si>
@@ -74,6 +74,51 @@
   </si>
   <si>
     <t>Breast Color</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>d1a2s</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>adsa2</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>12c</t>
+  </si>
+  <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>sda1</t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
 </sst>
 </file>
@@ -109,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +437,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -447,6 +493,181 @@
         <v>14</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1232</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45061.766585648147</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45061.801041666666</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>1232</v>
+      </c>
+      <c r="H3">
+        <v>1232</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>123111</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45061.869386574072</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>123112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45061.869756944441</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>111</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>122</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45061.871377314812</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>123</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -454,7 +675,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4950E8-1EF4-4576-9779-7941681CF811}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -486,6 +707,23 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>